<commit_message>
trying to get data out of everything
blah blah
</commit_message>
<xml_diff>
--- a/datasample.xlsx
+++ b/datasample.xlsx
@@ -314,15 +314,6 @@
     <xf numFmtId="46" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -336,6 +327,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,64 +471,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0428744632755831</c:v>
+                  <c:v>0.93511886970909719</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91792684640263988</c:v>
+                  <c:v>0.94011518967563412</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95209414176226115</c:v>
+                  <c:v>1.0113015982551752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0275080139262838</c:v>
+                  <c:v>1.0173050444723097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90617020756500732</c:v>
+                  <c:v>0.99965662853098913</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99190901467349024</c:v>
+                  <c:v>1.013047249154214</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0519262884520519</c:v>
+                  <c:v>0.91452228795661661</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0347149312604136</c:v>
+                  <c:v>0.90360504670629493</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0762745343192097</c:v>
+                  <c:v>0.93630964523861504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.98217194198764979</c:v>
+                  <c:v>1.0401548094942985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.91542025224997781</c:v>
+                  <c:v>1.0114375761941785</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.9915887311911693</c:v>
+                  <c:v>1.012516161276128</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.97359890379772307</c:v>
+                  <c:v>0.96859091004211229</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0895805579650557</c:v>
+                  <c:v>0.93790451741631686</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0432726240437595</c:v>
+                  <c:v>0.93607120950457545</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.97652668746000859</c:v>
+                  <c:v>0.97829645690232081</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.070328972637028</c:v>
+                  <c:v>0.90180008735064221</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99157266251702669</c:v>
+                  <c:v>0.98670105412445397</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.90247490759874793</c:v>
+                  <c:v>0.99380379934033802</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0793153646837612</c:v>
+                  <c:v>1.0238319110415597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -652,28 +652,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.9222899775088389</c:v>
+                  <c:v>2.0381291783216673</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0824901364768849</c:v>
+                  <c:v>2.0219607756775035</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.975264027142126</c:v>
+                  <c:v>1.9173649924682203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0845825968160461</c:v>
+                  <c:v>1.9680228811120357</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0881689916032595</c:v>
+                  <c:v>2.052403476600384</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0363570740113199</c:v>
+                  <c:v>2.0024183808987939</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0410992381222508</c:v>
+                  <c:v>2.0001220292318109</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9124217536650603</c:v>
+                  <c:v>2.0506551498194021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -761,28 +761,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.9850807680418403</c:v>
+                  <c:v>3.0976927786279957</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9188846028956439</c:v>
+                  <c:v>2.9227672214365348</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0144365162206883</c:v>
+                  <c:v>2.9546484652292313</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9149456493064605</c:v>
+                  <c:v>2.9799845678756536</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9783932975436778</c:v>
+                  <c:v>2.9755052323841822</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9336887064106083</c:v>
+                  <c:v>3.0946098049828188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0298102966512475</c:v>
+                  <c:v>2.9545806220358415</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9921081895899868</c:v>
+                  <c:v>3.0426565306921143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1539,64 +1539,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0428744632755831</c:v>
+                  <c:v>0.93511886970909719</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.91792684640263988</c:v>
+                  <c:v>0.94011518967563412</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95209414176226115</c:v>
+                  <c:v>1.0113015982551752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0275080139262838</c:v>
+                  <c:v>1.0173050444723097</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90617020756500732</c:v>
+                  <c:v>0.99965662853098913</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.99190901467349024</c:v>
+                  <c:v>1.013047249154214</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0519262884520519</c:v>
+                  <c:v>0.91452228795661661</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0347149312604136</c:v>
+                  <c:v>0.90360504670629493</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0762745343192097</c:v>
+                  <c:v>0.93630964523861504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.98217194198764979</c:v>
+                  <c:v>1.0401548094942985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.91542025224997781</c:v>
+                  <c:v>1.0114375761941785</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.9915887311911693</c:v>
+                  <c:v>1.012516161276128</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.97359890379772307</c:v>
+                  <c:v>0.96859091004211229</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0895805579650557</c:v>
+                  <c:v>0.93790451741631686</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0432726240437595</c:v>
+                  <c:v>0.93607120950457545</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.97652668746000859</c:v>
+                  <c:v>0.97829645690232081</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.070328972637028</c:v>
+                  <c:v>0.90180008735064221</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99157266251702669</c:v>
+                  <c:v>0.98670105412445397</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.90247490759874793</c:v>
+                  <c:v>0.99380379934033802</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0793153646837612</c:v>
+                  <c:v>1.0238319110415597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1720,28 +1720,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.9222899775088389</c:v>
+                  <c:v>2.0381291783216673</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0824901364768849</c:v>
+                  <c:v>2.0219607756775035</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.975264027142126</c:v>
+                  <c:v>1.9173649924682203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0845825968160461</c:v>
+                  <c:v>1.9680228811120357</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0881689916032595</c:v>
+                  <c:v>2.052403476600384</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0363570740113199</c:v>
+                  <c:v>2.0024183808987939</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0410992381222508</c:v>
+                  <c:v>2.0001220292318109</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9124217536650603</c:v>
+                  <c:v>2.0506551498194021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1829,28 +1829,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.9850807680418403</c:v>
+                  <c:v>3.0976927786279957</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9188846028956439</c:v>
+                  <c:v>2.9227672214365348</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0144365162206883</c:v>
+                  <c:v>2.9546484652292313</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.9149456493064605</c:v>
+                  <c:v>2.9799845678756536</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9783932975436778</c:v>
+                  <c:v>2.9755052323841822</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9336887064106083</c:v>
+                  <c:v>3.0946098049828188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0298102966512475</c:v>
+                  <c:v>2.9545806220358415</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9921081895899868</c:v>
+                  <c:v>3.0426565306921143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3998,16 +3998,16 @@
       <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
       <c r="AJ1" t="s">
         <v>14</v>
       </c>
@@ -4126,7 +4126,7 @@
       <c r="AO2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AP2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="AQ2" s="2" t="s">
@@ -4144,10 +4144,10 @@
       <c r="AU2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AV2" s="10" t="s">
+      <c r="AV2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AW2" s="11" t="s">
+      <c r="AW2" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -13968,7 +13968,7 @@
       <c r="AL69" s="3">
         <v>60300</v>
       </c>
-      <c r="AM69" s="9">
+      <c r="AM69" s="6">
         <v>0</v>
       </c>
       <c r="AN69" s="3">
@@ -18792,7 +18792,7 @@
       </c>
     </row>
     <row r="105" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D105" t="s">
@@ -18910,7 +18910,7 @@
       </c>
     </row>
     <row r="106" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
+      <c r="A106" s="13"/>
       <c r="D106" t="s">
         <v>27</v>
       </c>
@@ -19026,7 +19026,7 @@
       </c>
     </row>
     <row r="107" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
+      <c r="A107" s="13"/>
       <c r="D107" t="s">
         <v>28</v>
       </c>
@@ -19142,7 +19142,7 @@
       </c>
     </row>
     <row r="108" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A108" s="8"/>
+      <c r="A108" s="13"/>
       <c r="D108" t="s">
         <v>29</v>
       </c>
@@ -19282,7 +19282,7 @@
       </c>
     </row>
     <row r="110" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D110" t="s">
@@ -19390,7 +19390,7 @@
       </c>
     </row>
     <row r="111" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
+      <c r="A111" s="13"/>
       <c r="D111" t="s">
         <v>27</v>
       </c>
@@ -19496,7 +19496,7 @@
       </c>
     </row>
     <row r="112" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A112" s="8"/>
+      <c r="A112" s="13"/>
       <c r="D112" t="s">
         <v>28</v>
       </c>
@@ -19570,7 +19570,7 @@
       </c>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A113" s="8"/>
+      <c r="A113" s="13"/>
       <c r="D113" t="s">
         <v>29</v>
       </c>
@@ -19644,7 +19644,7 @@
       </c>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D115" t="s">
@@ -19720,7 +19720,7 @@
       </c>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
+      <c r="A116" s="13"/>
       <c r="D116" t="s">
         <v>27</v>
       </c>
@@ -19794,7 +19794,7 @@
       </c>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A117" s="8"/>
+      <c r="A117" s="13"/>
       <c r="D117" t="s">
         <v>28</v>
       </c>
@@ -19868,7 +19868,7 @@
       </c>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A118" s="8"/>
+      <c r="A118" s="13"/>
       <c r="D118" t="s">
         <v>29</v>
       </c>
@@ -19955,15 +19955,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U29"/>
+  <dimension ref="A2:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="W35" sqref="W35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3:Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -19974,7 +19974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>34</v>
       </c>
@@ -20002,14 +20002,23 @@
       <c r="U3" t="s">
         <v>35</v>
       </c>
+      <c r="W3">
+        <v>2.3876078342792253</v>
+      </c>
+      <c r="X3">
+        <v>9.1399700858036503</v>
+      </c>
+      <c r="Y3">
+        <v>18.668122183335434</v>
+      </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
         <f ca="1">B4+ (RAND()-0.5)/5</f>
-        <v>1.0428744632755831</v>
+        <v>0.93511886970909719</v>
       </c>
       <c r="D4">
         <v>8595.3882034052112</v>
@@ -20025,8 +20034,8 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <f ca="1">I4+ (RAND()-0.5)/5</f>
-        <v>1.9222899775088389</v>
+        <f t="shared" ref="J4:J11" ca="1" si="0">I4+ (RAND()-0.5)/5</f>
+        <v>2.0381291783216673</v>
       </c>
       <c r="K4">
         <v>32903.892308893141</v>
@@ -20043,7 +20052,7 @@
       </c>
       <c r="Q4">
         <f ca="1">P4+ (RAND()-0.5)/5</f>
-        <v>2.9850807680418403</v>
+        <v>3.0976927786279957</v>
       </c>
       <c r="R4">
         <v>6905.2398600075694</v>
@@ -20059,20 +20068,29 @@
       <c r="U4">
         <v>1.847956237915904E-3</v>
       </c>
+      <c r="W4">
+        <v>1.49555546519148</v>
+      </c>
+      <c r="X4">
+        <v>5.8033483750875803</v>
+      </c>
+      <c r="Y4">
+        <v>19.006891438710394</v>
+      </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C23" ca="1" si="0">B5+ (RAND()-0.5)/5</f>
-        <v>0.91792684640263988</v>
+        <f t="shared" ref="C5:C23" ca="1" si="1">B5+ (RAND()-0.5)/5</f>
+        <v>0.94011518967563412</v>
       </c>
       <c r="D5">
         <v>5383.9996746893275</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E23" si="1">D5/3600</f>
+        <f t="shared" ref="E5:E23" si="2">D5/3600</f>
         <v>1.49555546519148</v>
       </c>
       <c r="F5">
@@ -20082,14 +20100,14 @@
         <v>2</v>
       </c>
       <c r="J5">
-        <f ca="1">I5+ (RAND()-0.5)/5</f>
-        <v>2.0824901364768849</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0219607756775035</v>
       </c>
       <c r="K5">
         <v>20892.054150315289</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L11" si="2">K5/3600</f>
+        <f t="shared" ref="L5:L11" si="3">K5/3600</f>
         <v>5.8033483750875803</v>
       </c>
       <c r="M5">
@@ -20099,37 +20117,46 @@
         <v>3</v>
       </c>
       <c r="Q5">
-        <f t="shared" ref="Q5:Q12" ca="1" si="3">P5+ (RAND()-0.5)/5</f>
-        <v>2.9188846028956439</v>
+        <f t="shared" ref="Q5:Q12" ca="1" si="4">P5+ (RAND()-0.5)/5</f>
+        <v>2.9227672214365348</v>
       </c>
       <c r="R5">
         <v>8124.8091793574122</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S11" si="4">R5+60300</f>
+        <f t="shared" ref="S5:S11" si="5">R5+60300</f>
         <v>68424.809179357413</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:T11" si="5">S5/3600</f>
+        <f t="shared" ref="T5:T11" si="6">S5/3600</f>
         <v>19.006891438710394</v>
       </c>
       <c r="U5">
         <v>2.3939785934755579E-3</v>
       </c>
+      <c r="W5">
+        <v>2.4002494233398193</v>
+      </c>
+      <c r="X5">
+        <v>6.0090495291908725</v>
+      </c>
+      <c r="Y5">
+        <v>25.845002205773774</v>
+      </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95209414176226115</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0113015982551752</v>
       </c>
       <c r="D6">
         <v>8640.8979240233493</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4002494233398193</v>
       </c>
       <c r="F6">
@@ -20139,14 +20166,14 @@
         <v>2</v>
       </c>
       <c r="J6">
-        <f ca="1">I6+ (RAND()-0.5)/5</f>
-        <v>1.975264027142126</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9173649924682203</v>
       </c>
       <c r="K6">
         <v>21632.57830508714</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0090495291908725</v>
       </c>
       <c r="M6">
@@ -20156,37 +20183,46 @@
         <v>3</v>
       </c>
       <c r="Q6">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.0144365162206883</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2.9546484652292313</v>
       </c>
       <c r="R6">
         <v>32742.007940785588</v>
       </c>
       <c r="S6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>93042.007940785581</v>
       </c>
       <c r="T6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25.845002205773774</v>
       </c>
       <c r="U6">
         <v>8.9228605899109603E-4</v>
       </c>
+      <c r="W6">
+        <v>2.3511461449169273</v>
+      </c>
+      <c r="X6">
+        <v>5.0518500543271356</v>
+      </c>
+      <c r="Y6">
+        <v>19.979947831433719</v>
+      </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0275080139262838</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0173050444723097</v>
       </c>
       <c r="D7">
         <v>8464.1261217009378</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3511461449169273</v>
       </c>
       <c r="F7">
@@ -20196,14 +20232,14 @@
         <v>2</v>
       </c>
       <c r="J7">
-        <f ca="1">I7+ (RAND()-0.5)/5</f>
-        <v>2.0845825968160461</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9680228811120357</v>
       </c>
       <c r="K7">
         <v>18186.66019557769</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.0518500543271356</v>
       </c>
       <c r="M7">
@@ -20213,37 +20249,46 @@
         <v>3</v>
       </c>
       <c r="Q7">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.9149456493064605</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2.9799845678756536</v>
       </c>
       <c r="R7">
         <v>11627.81219316138</v>
       </c>
       <c r="S7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71927.812193161386</v>
       </c>
       <c r="T7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19.979947831433719</v>
       </c>
       <c r="U7">
         <v>2.0967429302643269E-3</v>
       </c>
+      <c r="W7">
+        <v>1.6168785308990552</v>
+      </c>
+      <c r="X7">
+        <v>5.1900247545802944</v>
+      </c>
+      <c r="Y7">
+        <v>22.149545632371503</v>
+      </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.90617020756500732</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99965662853098913</v>
       </c>
       <c r="D8">
         <v>5820.762711236599</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6168785308990552</v>
       </c>
       <c r="F8">
@@ -20253,14 +20298,14 @@
         <v>2</v>
       </c>
       <c r="J8">
-        <f ca="1">I8+ (RAND()-0.5)/5</f>
-        <v>2.0881689916032595</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.052403476600384</v>
       </c>
       <c r="K8">
         <v>18684.08911648906</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.1900247545802944</v>
       </c>
       <c r="M8">
@@ -20270,37 +20315,46 @@
         <v>3</v>
       </c>
       <c r="Q8">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.9783932975436778</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2.9755052323841822</v>
       </c>
       <c r="R8">
         <v>19438.36427653741</v>
       </c>
       <c r="S8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79738.36427653741</v>
       </c>
       <c r="T8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.149545632371503</v>
       </c>
       <c r="U8">
         <v>1.387914992101044E-3</v>
       </c>
+      <c r="W8">
+        <v>1.4441218198046168</v>
+      </c>
+      <c r="X8">
+        <v>5.3718364629404132</v>
+      </c>
+      <c r="Y8">
+        <v>24.038395528560116</v>
+      </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.99190901467349024</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.013047249154214</v>
       </c>
       <c r="D9">
         <v>5198.8385512966206</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4441218198046168</v>
       </c>
       <c r="F9">
@@ -20310,14 +20364,14 @@
         <v>2</v>
       </c>
       <c r="J9">
-        <f ca="1">I9+ (RAND()-0.5)/5</f>
-        <v>2.0363570740113199</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0024183808987939</v>
       </c>
       <c r="K9">
         <v>19338.611266585489</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.3718364629404132</v>
       </c>
       <c r="M9">
@@ -20327,37 +20381,46 @@
         <v>3</v>
       </c>
       <c r="Q9">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.9336887064106083</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.0946098049828188</v>
       </c>
       <c r="R9">
         <v>26238.223902816411</v>
       </c>
       <c r="S9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86538.223902816419</v>
       </c>
       <c r="T9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24.038395528560116</v>
       </c>
       <c r="U9">
         <v>1.3522831975875749E-3</v>
       </c>
+      <c r="W9">
+        <v>1.6808040352775282</v>
+      </c>
+      <c r="X9">
+        <v>5.4581859932570413</v>
+      </c>
+      <c r="Y9">
+        <v>20.648261786018434</v>
+      </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0519262884520519</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91452228795661661</v>
       </c>
       <c r="D10">
         <v>6050.8945269991018</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6808040352775282</v>
       </c>
       <c r="F10">
@@ -20367,14 +20430,14 @@
         <v>2</v>
       </c>
       <c r="J10">
-        <f ca="1">I10+ (RAND()-0.5)/5</f>
-        <v>2.0410992381222508</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0001220292318109</v>
       </c>
       <c r="K10">
         <v>19649.46957572535</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.4581859932570413</v>
       </c>
       <c r="M10">
@@ -20384,37 +20447,46 @@
         <v>3</v>
       </c>
       <c r="Q10">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.0298102966512475</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2.9545806220358415</v>
       </c>
       <c r="R10">
         <v>14033.74242966637</v>
       </c>
       <c r="S10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74333.742429666367</v>
       </c>
       <c r="T10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20.648261786018434</v>
       </c>
       <c r="U10">
         <v>1.576535917189872E-3</v>
       </c>
+      <c r="W10">
+        <v>1.7665505294004209</v>
+      </c>
+      <c r="X10">
+        <v>4.3227745870439609</v>
+      </c>
+      <c r="Y10">
+        <v>18.513184260307998</v>
+      </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0347149312604136</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90360504670629493</v>
       </c>
       <c r="D11">
         <v>6359.5819058415154</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7665505294004209</v>
       </c>
       <c r="F11">
@@ -20424,14 +20496,14 @@
         <v>2</v>
       </c>
       <c r="J11">
-        <f ca="1">I11+ (RAND()-0.5)/5</f>
-        <v>1.9124217536650603</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0506551498194021</v>
       </c>
       <c r="K11">
         <v>15561.988513358259</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.3227745870439609</v>
       </c>
       <c r="M11">
@@ -20441,37 +20513,40 @@
         <v>3</v>
       </c>
       <c r="Q11">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.9921081895899868</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.0426565306921143</v>
       </c>
       <c r="R11">
         <v>6347.4633371087957</v>
       </c>
       <c r="S11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66647.463337108798</v>
       </c>
       <c r="T11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>18.513184260307998</v>
       </c>
       <c r="U11">
         <v>2.0104802857965919E-3</v>
       </c>
+      <c r="W11">
+        <v>1.7642577164344562</v>
+      </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0762745343192097</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93630964523861504</v>
       </c>
       <c r="D12">
         <v>6351.3277791640421</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7642577164344562</v>
       </c>
       <c r="F12">
@@ -20485,19 +20560,19 @@
         <v>20856.167929003925</v>
       </c>
       <c r="L12">
-        <f t="shared" ref="L12:M12" si="6">AVERAGE(L4:L11)</f>
+        <f t="shared" ref="L12:M12" si="7">AVERAGE(L4:L11)</f>
         <v>5.7933799802788686</v>
       </c>
       <c r="M12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.6953613537186903E-4</v>
       </c>
       <c r="P12">
         <v>3</v>
       </c>
       <c r="Q12">
-        <f t="shared" ca="1" si="3"/>
-        <v>2.9924365646771727</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.0686772889410827</v>
       </c>
       <c r="R12" t="s">
         <v>38</v>
@@ -20514,20 +20589,23 @@
         <f>AVERAGE(U4:U11)</f>
         <v>1.6947722766652456E-3</v>
       </c>
+      <c r="W12">
+        <v>2.2875842532610422</v>
+      </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.98217194198764979</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0401548094942985</v>
       </c>
       <c r="D13">
         <v>8235.3033117397517</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2875842532610422</v>
       </c>
       <c r="F13">
@@ -20541,11 +20619,11 @@
         <v>5201.4200857327369</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:M13" si="7">STDEV(L4:L11)</f>
+        <f t="shared" ref="L13:M13" si="8">STDEV(L4:L11)</f>
         <v>1.4448389127035368</v>
       </c>
       <c r="M13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.673152829538485E-4</v>
       </c>
       <c r="R13" t="s">
@@ -20563,20 +20641,23 @@
         <f>STDEV(U4:U11)</f>
         <v>4.844777573359609E-4</v>
       </c>
+      <c r="W13">
+        <v>1.4896523749020205</v>
+      </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.91542025224997781</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0114375761941785</v>
       </c>
       <c r="D14">
         <v>5362.7485496472736</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4896523749020205</v>
       </c>
       <c r="F14">
@@ -20594,20 +20675,23 @@
       <c r="S14">
         <v>1.6949999999999999E-3</v>
       </c>
+      <c r="W14">
+        <v>1.5159411175576876</v>
+      </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.9915887311911693</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.012516161276128</v>
       </c>
       <c r="D15">
         <v>5457.3880232076754</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5159411175576876</v>
       </c>
       <c r="F15">
@@ -20640,20 +20724,23 @@
       <c r="T15">
         <v>4.84E-4</v>
       </c>
+      <c r="W15">
+        <v>1.4508416298230684</v>
+      </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.97359890379772307</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96859091004211229</v>
       </c>
       <c r="D16">
         <v>5223.0298673630459</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4508416298230684</v>
       </c>
       <c r="F16">
@@ -20683,20 +20770,23 @@
       <c r="S16">
         <v>1.6949999999999999E-3</v>
       </c>
+      <c r="W16">
+        <v>2.2547740482552117</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0895805579650557</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93790451741631686</v>
       </c>
       <c r="D17">
         <v>8117.1865737187618</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2547740482552117</v>
       </c>
       <c r="F17">
@@ -20711,124 +20801,142 @@
       <c r="L17">
         <v>5.6999999999999998E-4</v>
       </c>
+      <c r="W17">
+        <v>4.4727591757336667</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0432726240437595</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93607120950457545</v>
       </c>
       <c r="D18">
         <v>16101.9330326412</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.4727591757336667</v>
       </c>
       <c r="F18">
         <v>1.93010559918264E-3</v>
       </c>
+      <c r="W18">
+        <v>1.5503805173191234</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.97652668746000859</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.97829645690232081</v>
       </c>
       <c r="D19">
         <v>5581.3698623488444</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5503805173191234</v>
       </c>
       <c r="F19">
         <v>2.4467015368269448E-3</v>
       </c>
+      <c r="W19">
+        <v>2.8199806462630304</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.070328972637028</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90180008735064221</v>
       </c>
       <c r="D20">
         <v>10151.93032654691</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.8199806462630304</v>
       </c>
       <c r="F20">
         <v>2.0740295065557151E-3</v>
       </c>
+      <c r="W20">
+        <v>3.6315578243796334</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.99157266251702669</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98670105412445397</v>
       </c>
       <c r="D21">
         <v>13073.608167766681</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6315578243796334</v>
       </c>
       <c r="F21">
         <v>2.0727442370196531E-3</v>
       </c>
+      <c r="W21">
+        <v>3.2533584241729336</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.90247490759874793</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99380379934033802</v>
       </c>
       <c r="D22">
         <v>11712.090327022561</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2533584241729336</v>
       </c>
       <c r="F22">
         <v>2.2114693074936969E-3</v>
       </c>
-      <c r="U22" s="13"/>
+      <c r="U22" s="10"/>
+      <c r="W22">
+        <v>2.7435422119198782</v>
+      </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.0793153646837612</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0238319110415597</v>
       </c>
       <c r="D23">
         <v>9876.7519629115613</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7435422119198782</v>
       </c>
       <c r="F23">
         <v>2.5404661183147312E-3</v>
       </c>
-      <c r="U23" s="13"/>
+      <c r="U23" s="10"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>38</v>
       </c>
@@ -20837,16 +20945,16 @@
         <v>7987.9578701635492</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:F24" si="8">AVERAGE(E4:E23)</f>
+        <f t="shared" ref="E24:F24" si="9">AVERAGE(E4:E23)</f>
         <v>2.2188771861565417</v>
       </c>
       <c r="F24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.4334364735870101E-3</v>
       </c>
-      <c r="U24" s="13"/>
+      <c r="U24" s="10"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -20855,19 +20963,19 @@
         <v>2991.1336839184155</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25:F25" si="9">STDEV(E4:E23)</f>
+        <f t="shared" ref="E25:F25" si="10">STDEV(E4:E23)</f>
         <v>0.83087046775511408</v>
       </c>
       <c r="F25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.1950481131008137E-4</v>
       </c>
-      <c r="U25" s="13"/>
+      <c r="U25" s="10"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U26" s="13"/>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U26" s="10"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -20880,9 +20988,9 @@
       <c r="E27">
         <v>2.4334364735870101E-3</v>
       </c>
-      <c r="U27" s="13"/>
+      <c r="U27" s="10"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>1</v>
       </c>
@@ -20898,9 +21006,9 @@
       <c r="F28">
         <v>3.1950481131008137E-4</v>
       </c>
-      <c r="U28" s="13"/>
+      <c r="U28" s="10"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>1.1000000000000001</v>
       </c>
@@ -20910,7 +21018,7 @@
       <c r="E29">
         <v>2.4334364735870101E-3</v>
       </c>
-      <c r="U29" s="13"/>
+      <c r="U29" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>